<commit_message>
write time of wells
</commit_message>
<xml_diff>
--- a/templates/template.xlsx
+++ b/templates/template.xlsx
@@ -482,7 +482,7 @@
       <alignment horizontal="center" vertical="center" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
-    <xf numFmtId="164" fontId="6" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="false">
+    <xf numFmtId="164" fontId="6" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
       <alignment horizontal="left" vertical="center" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
@@ -683,13 +683,17 @@
       <protection locked="true" hidden="false"/>
     </xf>
     <xf numFmtId="165" fontId="11" fillId="0" borderId="4" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
-      <alignment horizontal="center" vertical="center" textRotation="0" wrapText="true" indent="0" shrinkToFit="false"/>
+      <alignment horizontal="left" vertical="center" textRotation="0" wrapText="true" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
     <xf numFmtId="166" fontId="12" fillId="3" borderId="4" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
       <alignment horizontal="center" vertical="center" textRotation="0" wrapText="true" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
+    <xf numFmtId="165" fontId="11" fillId="0" borderId="12" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
+      <alignment horizontal="left" vertical="center" textRotation="0" wrapText="true" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
+    </xf>
     <xf numFmtId="164" fontId="13" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="false">
       <alignment horizontal="general" vertical="center" textRotation="0" wrapText="true" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
@@ -731,11 +735,7 @@
       <protection locked="true" hidden="false"/>
     </xf>
     <xf numFmtId="166" fontId="8" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
-      <alignment horizontal="right" vertical="center" textRotation="0" wrapText="true" indent="2" shrinkToFit="false"/>
-      <protection locked="true" hidden="false"/>
-    </xf>
-    <xf numFmtId="164" fontId="6" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
-      <alignment horizontal="left" vertical="center" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
+      <alignment horizontal="right" vertical="center" textRotation="0" wrapText="true" indent="4" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
     <xf numFmtId="164" fontId="6" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="false">
@@ -853,11 +853,11 @@
   </sheetPr>
   <dimension ref="A1:AL39"/>
   <sheetViews>
-    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A4" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="AD21" activeCellId="0" sqref="AD21"/>
+    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
+      <selection pane="topLeft" activeCell="D23" activeCellId="0" sqref="D23"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="8.5390625" defaultRowHeight="15" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
+  <sheetFormatPr defaultColWidth="8.54296875" defaultRowHeight="15" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
   <cols>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1" min="1" style="0" width="10.28"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="2" min="2" style="0" width="13.43"/>
@@ -873,21 +873,21 @@
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="13" min="13" style="0" width="8"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="14" min="14" style="0" width="9"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="15" min="15" style="0" width="8.14"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="16" min="16" style="0" width="8.71"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="16" min="16" style="0" width="8.7"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="17" min="17" style="0" width="8.28"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="19" min="19" style="0" width="8.28"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="21" min="20" style="0" width="8.14"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="22" min="22" style="0" width="7.85"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="23" min="23" style="0" width="8.71"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="23" min="23" style="0" width="8.7"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="24" min="24" style="0" width="8.85"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="26" min="25" style="0" width="8.28"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="28" min="27" style="0" width="8"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="29" min="29" style="0" width="8.28"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="31" min="30" style="0" width="7.71"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="32" min="32" style="0" width="8.71"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="31" min="30" style="0" width="7.7"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="32" min="32" style="0" width="8.7"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="33" min="33" style="0" width="8.85"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="34" min="34" style="0" width="7.71"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="35" min="35" style="0" width="6.71"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="34" min="34" style="0" width="7.7"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="35" min="35" style="0" width="6.7"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="36" min="36" style="0" width="10.43"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="37" min="37" style="0" width="8.14"/>
   </cols>
@@ -2081,7 +2081,7 @@
       </c>
       <c r="AL17" s="22"/>
     </row>
-    <row r="18" customFormat="false" ht="25.5" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="18" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A18" s="37"/>
       <c r="B18" s="38" t="s">
         <v>14</v>
@@ -2135,7 +2135,7 @@
       </c>
       <c r="AL18" s="22"/>
     </row>
-    <row r="19" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="19" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A19" s="37"/>
       <c r="B19" s="24" t="s">
         <v>12</v>
@@ -2143,7 +2143,7 @@
       <c r="C19" s="25" t="n">
         <v>44559</v>
       </c>
-      <c r="D19" s="52" t="s">
+      <c r="D19" s="55" t="s">
         <v>15</v>
       </c>
       <c r="E19" s="46"/>
@@ -2335,199 +2335,199 @@
       <c r="AL20" s="22"/>
     </row>
     <row r="21" customFormat="false" ht="14.15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A21" s="55"/>
-      <c r="B21" s="56"/>
-      <c r="C21" s="57"/>
-      <c r="D21" s="57"/>
-      <c r="E21" s="58"/>
-      <c r="F21" s="58"/>
-      <c r="G21" s="58"/>
-      <c r="H21" s="58"/>
-      <c r="I21" s="58"/>
-      <c r="J21" s="58"/>
-      <c r="K21" s="58"/>
-      <c r="L21" s="58"/>
-      <c r="M21" s="58"/>
-      <c r="N21" s="58"/>
-      <c r="O21" s="58"/>
-      <c r="P21" s="58"/>
-      <c r="Q21" s="58"/>
-      <c r="R21" s="58"/>
-      <c r="S21" s="58"/>
-      <c r="T21" s="58"/>
-      <c r="U21" s="58"/>
-      <c r="V21" s="58"/>
-      <c r="W21" s="58"/>
-      <c r="X21" s="58"/>
-      <c r="Y21" s="58"/>
-      <c r="Z21" s="58"/>
-      <c r="AA21" s="58"/>
-      <c r="AB21" s="58"/>
-      <c r="AC21" s="58"/>
-      <c r="AD21" s="59"/>
-      <c r="AE21" s="59"/>
-      <c r="AF21" s="59"/>
-      <c r="AG21" s="59"/>
-      <c r="AH21" s="59" t="s">
+      <c r="A21" s="56"/>
+      <c r="B21" s="57"/>
+      <c r="C21" s="58"/>
+      <c r="D21" s="58"/>
+      <c r="E21" s="59"/>
+      <c r="F21" s="59"/>
+      <c r="G21" s="59"/>
+      <c r="H21" s="59"/>
+      <c r="I21" s="59"/>
+      <c r="J21" s="59"/>
+      <c r="K21" s="59"/>
+      <c r="L21" s="59"/>
+      <c r="M21" s="59"/>
+      <c r="N21" s="59"/>
+      <c r="O21" s="59"/>
+      <c r="P21" s="59"/>
+      <c r="Q21" s="59"/>
+      <c r="R21" s="59"/>
+      <c r="S21" s="59"/>
+      <c r="T21" s="59"/>
+      <c r="U21" s="59"/>
+      <c r="V21" s="59"/>
+      <c r="W21" s="59"/>
+      <c r="X21" s="59"/>
+      <c r="Y21" s="59"/>
+      <c r="Z21" s="59"/>
+      <c r="AA21" s="59"/>
+      <c r="AB21" s="59"/>
+      <c r="AC21" s="59"/>
+      <c r="AD21" s="60"/>
+      <c r="AE21" s="60"/>
+      <c r="AF21" s="60"/>
+      <c r="AG21" s="60"/>
+      <c r="AH21" s="60" t="s">
         <v>16</v>
       </c>
-      <c r="AI21" s="59"/>
-      <c r="AJ21" s="60" t="n">
+      <c r="AI21" s="60"/>
+      <c r="AJ21" s="61" t="n">
         <f aca="false">AJ11+AJ14+AJ17+AJ20</f>
         <v>381971</v>
       </c>
-      <c r="AK21" s="60" t="n">
+      <c r="AK21" s="61" t="n">
         <f aca="false">AK11+AK14+AK17+AK20</f>
         <v>0</v>
       </c>
-      <c r="AL21" s="61"/>
+      <c r="AL21" s="62"/>
     </row>
     <row r="22" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A22" s="55"/>
-      <c r="B22" s="56"/>
-      <c r="C22" s="57"/>
-      <c r="D22" s="57"/>
-      <c r="AJ22" s="62"/>
-      <c r="AK22" s="62"/>
-      <c r="AL22" s="61"/>
+      <c r="A22" s="56"/>
+      <c r="B22" s="57"/>
+      <c r="C22" s="58"/>
+      <c r="D22" s="58"/>
+      <c r="AJ22" s="63"/>
+      <c r="AK22" s="63"/>
+      <c r="AL22" s="62"/>
     </row>
     <row r="23" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A23" s="55"/>
-      <c r="B23" s="56"/>
-      <c r="C23" s="57"/>
-      <c r="D23" s="57"/>
-      <c r="E23" s="58"/>
-      <c r="F23" s="58"/>
-      <c r="G23" s="58"/>
-      <c r="H23" s="58"/>
-      <c r="I23" s="58"/>
-      <c r="J23" s="58"/>
-      <c r="K23" s="58"/>
-      <c r="L23" s="58"/>
-      <c r="M23" s="58"/>
-      <c r="N23" s="58"/>
-      <c r="O23" s="58"/>
-      <c r="P23" s="58"/>
-      <c r="Q23" s="58"/>
-      <c r="R23" s="58"/>
-      <c r="S23" s="58"/>
-      <c r="T23" s="58"/>
-      <c r="U23" s="58"/>
-      <c r="V23" s="58"/>
-      <c r="W23" s="58"/>
-      <c r="X23" s="58"/>
-      <c r="Y23" s="58"/>
-      <c r="Z23" s="58"/>
-      <c r="AA23" s="58"/>
-      <c r="AB23" s="58"/>
-      <c r="AC23" s="58"/>
-      <c r="AD23" s="58"/>
-      <c r="AE23" s="58"/>
-      <c r="AF23" s="58"/>
-      <c r="AG23" s="58"/>
-      <c r="AH23" s="58"/>
-      <c r="AI23" s="58"/>
-      <c r="AJ23" s="58"/>
-      <c r="AK23" s="62"/>
-      <c r="AL23" s="61"/>
+      <c r="A23" s="56"/>
+      <c r="B23" s="57"/>
+      <c r="C23" s="58"/>
+      <c r="D23" s="58"/>
+      <c r="E23" s="59"/>
+      <c r="F23" s="59"/>
+      <c r="G23" s="59"/>
+      <c r="H23" s="59"/>
+      <c r="I23" s="59"/>
+      <c r="J23" s="59"/>
+      <c r="K23" s="59"/>
+      <c r="L23" s="59"/>
+      <c r="M23" s="59"/>
+      <c r="N23" s="59"/>
+      <c r="O23" s="59"/>
+      <c r="P23" s="59"/>
+      <c r="Q23" s="59"/>
+      <c r="R23" s="59"/>
+      <c r="S23" s="59"/>
+      <c r="T23" s="59"/>
+      <c r="U23" s="59"/>
+      <c r="V23" s="59"/>
+      <c r="W23" s="59"/>
+      <c r="X23" s="59"/>
+      <c r="Y23" s="59"/>
+      <c r="Z23" s="59"/>
+      <c r="AA23" s="59"/>
+      <c r="AB23" s="59"/>
+      <c r="AC23" s="59"/>
+      <c r="AD23" s="59"/>
+      <c r="AE23" s="59"/>
+      <c r="AF23" s="59"/>
+      <c r="AG23" s="59"/>
+      <c r="AH23" s="59"/>
+      <c r="AI23" s="59"/>
+      <c r="AJ23" s="59"/>
+      <c r="AK23" s="63"/>
+      <c r="AL23" s="62"/>
     </row>
     <row r="24" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A24" s="55"/>
-      <c r="B24" s="56"/>
-      <c r="C24" s="57"/>
-      <c r="D24" s="57"/>
-      <c r="E24" s="63"/>
-      <c r="F24" s="63"/>
-      <c r="G24" s="63"/>
-      <c r="H24" s="63"/>
-      <c r="I24" s="63"/>
-      <c r="J24" s="63"/>
-      <c r="K24" s="63"/>
-      <c r="L24" s="63"/>
-      <c r="M24" s="63"/>
-      <c r="N24" s="63"/>
-      <c r="O24" s="63"/>
-      <c r="P24" s="63"/>
-      <c r="Q24" s="63"/>
-      <c r="R24" s="63"/>
-      <c r="S24" s="63"/>
-      <c r="T24" s="63"/>
-      <c r="U24" s="63"/>
-      <c r="V24" s="63"/>
-      <c r="W24" s="63"/>
-      <c r="X24" s="63"/>
-      <c r="Y24" s="63"/>
-      <c r="Z24" s="63"/>
-      <c r="AA24" s="63"/>
-      <c r="AB24" s="63"/>
-      <c r="AC24" s="63"/>
-      <c r="AD24" s="63"/>
-      <c r="AE24" s="63"/>
-      <c r="AF24" s="63"/>
-      <c r="AG24" s="63"/>
-      <c r="AH24" s="63"/>
-      <c r="AI24" s="63"/>
-      <c r="AJ24" s="63"/>
-      <c r="AK24" s="62"/>
-      <c r="AL24" s="61"/>
+      <c r="A24" s="56"/>
+      <c r="B24" s="57"/>
+      <c r="C24" s="58"/>
+      <c r="D24" s="58"/>
+      <c r="E24" s="64"/>
+      <c r="F24" s="64"/>
+      <c r="G24" s="64"/>
+      <c r="H24" s="64"/>
+      <c r="I24" s="64"/>
+      <c r="J24" s="64"/>
+      <c r="K24" s="64"/>
+      <c r="L24" s="64"/>
+      <c r="M24" s="64"/>
+      <c r="N24" s="64"/>
+      <c r="O24" s="64"/>
+      <c r="P24" s="64"/>
+      <c r="Q24" s="64"/>
+      <c r="R24" s="64"/>
+      <c r="S24" s="64"/>
+      <c r="T24" s="64"/>
+      <c r="U24" s="64"/>
+      <c r="V24" s="64"/>
+      <c r="W24" s="64"/>
+      <c r="X24" s="64"/>
+      <c r="Y24" s="64"/>
+      <c r="Z24" s="64"/>
+      <c r="AA24" s="64"/>
+      <c r="AB24" s="64"/>
+      <c r="AC24" s="64"/>
+      <c r="AD24" s="64"/>
+      <c r="AE24" s="64"/>
+      <c r="AF24" s="64"/>
+      <c r="AG24" s="64"/>
+      <c r="AH24" s="64"/>
+      <c r="AI24" s="64"/>
+      <c r="AJ24" s="64"/>
+      <c r="AK24" s="63"/>
+      <c r="AL24" s="62"/>
     </row>
     <row r="25" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A25" s="55"/>
-      <c r="B25" s="56"/>
-      <c r="C25" s="57"/>
-      <c r="D25" s="57"/>
-      <c r="E25" s="58"/>
-      <c r="F25" s="58"/>
-      <c r="G25" s="58"/>
-      <c r="H25" s="58"/>
-      <c r="I25" s="58"/>
-      <c r="J25" s="58"/>
-      <c r="K25" s="58"/>
-      <c r="L25" s="58"/>
-      <c r="M25" s="58"/>
-      <c r="N25" s="58"/>
-      <c r="O25" s="58"/>
-      <c r="P25" s="58"/>
-      <c r="Q25" s="58"/>
-      <c r="R25" s="58"/>
-      <c r="S25" s="58"/>
-      <c r="T25" s="58"/>
-      <c r="U25" s="58"/>
-      <c r="V25" s="58"/>
-      <c r="W25" s="58"/>
-      <c r="X25" s="58"/>
-      <c r="Y25" s="58"/>
-      <c r="Z25" s="58"/>
-      <c r="AA25" s="58"/>
-      <c r="AB25" s="58"/>
-      <c r="AC25" s="58"/>
-      <c r="AD25" s="58"/>
-      <c r="AE25" s="58"/>
-      <c r="AF25" s="58"/>
-      <c r="AG25" s="58"/>
-      <c r="AH25" s="58"/>
-      <c r="AI25" s="58"/>
-      <c r="AJ25" s="58"/>
-      <c r="AK25" s="62"/>
-      <c r="AL25" s="61"/>
+      <c r="A25" s="56"/>
+      <c r="B25" s="57"/>
+      <c r="C25" s="58"/>
+      <c r="D25" s="58"/>
+      <c r="E25" s="59"/>
+      <c r="F25" s="59"/>
+      <c r="G25" s="59"/>
+      <c r="H25" s="59"/>
+      <c r="I25" s="59"/>
+      <c r="J25" s="59"/>
+      <c r="K25" s="59"/>
+      <c r="L25" s="59"/>
+      <c r="M25" s="59"/>
+      <c r="N25" s="59"/>
+      <c r="O25" s="59"/>
+      <c r="P25" s="59"/>
+      <c r="Q25" s="59"/>
+      <c r="R25" s="59"/>
+      <c r="S25" s="59"/>
+      <c r="T25" s="59"/>
+      <c r="U25" s="59"/>
+      <c r="V25" s="59"/>
+      <c r="W25" s="59"/>
+      <c r="X25" s="59"/>
+      <c r="Y25" s="59"/>
+      <c r="Z25" s="59"/>
+      <c r="AA25" s="59"/>
+      <c r="AB25" s="59"/>
+      <c r="AC25" s="59"/>
+      <c r="AD25" s="59"/>
+      <c r="AE25" s="59"/>
+      <c r="AF25" s="59"/>
+      <c r="AG25" s="59"/>
+      <c r="AH25" s="59"/>
+      <c r="AI25" s="59"/>
+      <c r="AJ25" s="59"/>
+      <c r="AK25" s="63"/>
+      <c r="AL25" s="62"/>
     </row>
     <row r="26" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A26" s="64"/>
-      <c r="B26" s="56"/>
-      <c r="C26" s="57"/>
-      <c r="D26" s="57"/>
-      <c r="AI26" s="58"/>
-      <c r="AJ26" s="65"/>
-      <c r="AK26" s="65"/>
-      <c r="AL26" s="64"/>
+      <c r="A26" s="65"/>
+      <c r="B26" s="57"/>
+      <c r="C26" s="58"/>
+      <c r="D26" s="58"/>
+      <c r="AI26" s="59"/>
+      <c r="AJ26" s="66"/>
+      <c r="AK26" s="66"/>
+      <c r="AL26" s="65"/>
     </row>
     <row r="27" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A27" s="12"/>
-      <c r="B27" s="66" t="s">
+      <c r="B27" s="3" t="s">
         <v>17</v>
       </c>
-      <c r="C27" s="66"/>
-      <c r="D27" s="66"/>
+      <c r="C27" s="3"/>
+      <c r="D27" s="3"/>
       <c r="E27" s="67"/>
       <c r="F27" s="67"/>
       <c r="G27" s="67"/>

</xml_diff>

<commit_message>
add formules and printGuide
</commit_message>
<xml_diff>
--- a/templates/template.xlsx
+++ b/templates/template.xlsx
@@ -720,7 +720,7 @@
       <protection locked="true" hidden="false"/>
     </xf>
     <xf numFmtId="166" fontId="8" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
-      <alignment horizontal="right" vertical="center" textRotation="0" wrapText="true" indent="13" shrinkToFit="false"/>
+      <alignment horizontal="right" vertical="center" textRotation="0" wrapText="true" indent="15" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
     <xf numFmtId="164" fontId="6" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="false">
@@ -838,8 +838,8 @@
   </sheetPr>
   <dimension ref="A1:AL40"/>
   <sheetViews>
-    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="D17" activeCellId="0" sqref="D17"/>
+    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="S1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
+      <selection pane="topLeft" activeCell="AJ10" activeCellId="0" sqref="AJ10"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="8.54296875" defaultRowHeight="15" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
@@ -2341,7 +2341,9 @@
         <f aca="false">AK12+AK15+AK18+AK21</f>
         <v>#DIV/0!</v>
       </c>
-      <c r="AL22" s="60"/>
+      <c r="AL22" s="60" t="n">
+        <v>701</v>
+      </c>
     </row>
     <row r="23" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A23" s="54"/>

</xml_diff>